<commit_message>
1. Implement Previous data in week form
</commit_message>
<xml_diff>
--- a/report_template/weekMaintance.xlsx
+++ b/report_template/weekMaintance.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\AQM\report_template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="157">
   <si>
     <t>psi, 30±5</t>
   </si>
@@ -1918,40 +1923,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>YES☑  NO□</t>
-  </si>
-  <si>
     <t>2022/5/22</t>
-  </si>
-  <si>
-    <r>
-      <t>YES☑  NO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>□</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>YES☑  NO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>□</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">溫度 </t>
@@ -1990,14 +1962,22 @@
   </si>
   <si>
     <t>有效期限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前期數據</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上次保養日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="32">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2380,7 +2360,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2464,45 +2444,75 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2512,31 +2522,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2553,11 +2542,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2599,7 +2596,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2631,9 +2628,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2665,6 +2680,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2840,14 +2873,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F114" sqref="F114"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
@@ -2856,100 +2889,96 @@
     <col min="7" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.1" customHeight="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-    </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+    </row>
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56" t="s">
+        <v>156</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="28"/>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="8" t="s">
-        <v>152</v>
-      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="30"/>
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="42"/>
       <c r="B5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-    </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="30" t="s">
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="45"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="30"/>
-      <c r="B8" s="29" t="s">
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="42"/>
+      <c r="B8" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="30"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="42"/>
       <c r="B9" s="7" t="s">
         <v>115</v>
       </c>
@@ -2957,45 +2986,42 @@
       <c r="D9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E9" s="8"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="30" t="s">
+    <row r="10" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="45"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="42" t="s">
         <v>116</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="30"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="42"/>
       <c r="B12" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="30"/>
+      <c r="F12" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="42"/>
       <c r="B13" s="17" t="s">
         <v>85</v>
       </c>
@@ -3003,13 +3029,11 @@
       <c r="D13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E13" s="8"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="30"/>
+    <row r="14" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="42"/>
       <c r="B14" s="17" t="s">
         <v>119</v>
       </c>
@@ -3017,13 +3041,11 @@
       <c r="D14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E14" s="8"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="30"/>
+    <row r="15" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="42"/>
       <c r="B15" s="17" t="s">
         <v>120</v>
       </c>
@@ -3031,13 +3053,11 @@
       <c r="D15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="30"/>
+    <row r="16" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="42"/>
       <c r="B16" s="17" t="s">
         <v>121</v>
       </c>
@@ -3045,13 +3065,11 @@
       <c r="D16" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E16" s="8"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="30"/>
+    <row r="17" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="42"/>
       <c r="B17" s="17" t="s">
         <v>123</v>
       </c>
@@ -3059,13 +3077,11 @@
       <c r="D17" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>151</v>
-      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="30"/>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="42"/>
       <c r="B18" s="17" t="s">
         <v>125</v>
       </c>
@@ -3073,13 +3089,11 @@
       <c r="D18" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="30"/>
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="42"/>
       <c r="B19" s="17" t="s">
         <v>127</v>
       </c>
@@ -3087,13 +3101,11 @@
       <c r="D19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E19" s="8"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="30"/>
+    <row r="20" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="42"/>
       <c r="B20" s="17" t="s">
         <v>128</v>
       </c>
@@ -3101,13 +3113,11 @@
       <c r="D20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E20" s="8"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="30"/>
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="42"/>
       <c r="B21" s="17" t="s">
         <v>129</v>
       </c>
@@ -3115,13 +3125,11 @@
       <c r="D21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="30"/>
+    <row r="22" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="42"/>
       <c r="B22" s="17" t="s">
         <v>130</v>
       </c>
@@ -3129,13 +3137,11 @@
       <c r="D22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E22" s="8"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="30"/>
+    <row r="23" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="42"/>
       <c r="B23" s="17" t="s">
         <v>131</v>
       </c>
@@ -3143,57 +3149,53 @@
       <c r="D23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="30"/>
+    <row r="24" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="42"/>
       <c r="B24" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-    </row>
-    <row r="26" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="30" t="s">
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+    </row>
+    <row r="26" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="42" t="s">
         <v>133</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="30"/>
+    <row r="27" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="42"/>
       <c r="B27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="30"/>
+      <c r="F27" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="42"/>
       <c r="B28" s="17" t="s">
         <v>134</v>
       </c>
@@ -3201,13 +3203,11 @@
       <c r="D28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E28" s="8"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="30"/>
+    <row r="29" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="42"/>
       <c r="B29" s="17" t="s">
         <v>135</v>
       </c>
@@ -3215,13 +3215,11 @@
       <c r="D29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E29" s="8"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="30"/>
+    <row r="30" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="42"/>
       <c r="B30" s="17" t="s">
         <v>136</v>
       </c>
@@ -3229,13 +3227,11 @@
       <c r="D30" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E30" s="8"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="30"/>
+    <row r="31" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="42"/>
       <c r="B31" s="17" t="s">
         <v>137</v>
       </c>
@@ -3243,13 +3239,11 @@
       <c r="D31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="30"/>
+    <row r="32" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="42"/>
       <c r="B32" s="17" t="s">
         <v>138</v>
       </c>
@@ -3257,13 +3251,11 @@
       <c r="D32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="30"/>
+    <row r="33" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="42"/>
       <c r="B33" s="17" t="s">
         <v>139</v>
       </c>
@@ -3271,13 +3263,11 @@
       <c r="D33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="30"/>
+    <row r="34" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="42"/>
       <c r="B34" s="17" t="s">
         <v>140</v>
       </c>
@@ -3285,13 +3275,11 @@
       <c r="D34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E34" s="8"/>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="30"/>
+    <row r="35" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="42"/>
       <c r="B35" s="17" t="s">
         <v>141</v>
       </c>
@@ -3299,13 +3287,11 @@
       <c r="D35" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E35" s="8"/>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="30"/>
+    <row r="36" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="42"/>
       <c r="B36" s="17" t="s">
         <v>142</v>
       </c>
@@ -3313,13 +3299,11 @@
       <c r="D36" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E36" s="8"/>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="30"/>
+    <row r="37" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="42"/>
       <c r="B37" s="17" t="s">
         <v>144</v>
       </c>
@@ -3327,84 +3311,80 @@
       <c r="D37" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E37" s="8"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="30"/>
+    <row r="38" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="42"/>
       <c r="B38" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="8"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" s="5" customFormat="1" ht="15" customHeight="1"/>
-    <row r="40" spans="1:6" ht="15" customHeight="1"/>
-    <row r="41" spans="1:6" ht="15" customHeight="1"/>
-    <row r="42" spans="1:6" ht="26.1" customHeight="1">
-      <c r="A42" s="33" t="s">
+    <row r="39" spans="1:6" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-    </row>
-    <row r="43" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+    </row>
+    <row r="43" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
       <c r="D43" s="4"/>
       <c r="E43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="28"/>
     </row>
-    <row r="44" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
+    <row r="44" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
       <c r="E44" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A45" s="30" t="s">
+    <row r="45" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="42" t="s">
         <v>82</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="8"/>
       <c r="F45" s="7"/>
     </row>
-    <row r="46" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="30"/>
+    <row r="46" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="42"/>
       <c r="B46" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="8"/>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A47" s="30"/>
+      <c r="F46" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="42"/>
       <c r="B47" s="17" t="s">
         <v>85</v>
       </c>
@@ -3412,13 +3392,11 @@
       <c r="D47" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E47" s="8"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A48" s="30"/>
+    <row r="48" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="42"/>
       <c r="B48" s="17" t="s">
         <v>86</v>
       </c>
@@ -3426,13 +3404,11 @@
       <c r="D48" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E48" s="8"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="30"/>
+    <row r="49" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="42"/>
       <c r="B49" s="17" t="s">
         <v>88</v>
       </c>
@@ -3440,13 +3416,11 @@
       <c r="D49" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E49" s="8"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A50" s="30"/>
+    <row r="50" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="42"/>
       <c r="B50" s="17" t="s">
         <v>90</v>
       </c>
@@ -3454,13 +3428,11 @@
       <c r="D50" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E50" s="8"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A51" s="30"/>
+    <row r="51" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="42"/>
       <c r="B51" s="17" t="s">
         <v>91</v>
       </c>
@@ -3468,69 +3440,63 @@
       <c r="D51" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E51" s="8"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="30"/>
+    <row r="52" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="42"/>
       <c r="B52" s="17" t="s">
         <v>92</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
-      <c r="E52" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E52" s="8"/>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="30"/>
+    <row r="53" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="42"/>
       <c r="B53" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-    </row>
-    <row r="55" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A55" s="30" t="s">
+    <row r="54" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+    </row>
+    <row r="55" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="42" t="s">
         <v>94</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="8"/>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A56" s="30"/>
+    <row r="56" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="42"/>
       <c r="B56" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="8"/>
-      <c r="F56" s="7"/>
-    </row>
-    <row r="57" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A57" s="30"/>
+      <c r="F56" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="42"/>
       <c r="B57" s="17" t="s">
         <v>95</v>
       </c>
@@ -3538,13 +3504,11 @@
       <c r="D57" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E57" s="8"/>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A58" s="30"/>
+    <row r="58" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="42"/>
       <c r="B58" s="17" t="s">
         <v>96</v>
       </c>
@@ -3552,13 +3516,11 @@
       <c r="D58" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E58" s="8"/>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A59" s="30"/>
+    <row r="59" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="42"/>
       <c r="B59" s="17" t="s">
         <v>97</v>
       </c>
@@ -3566,13 +3528,11 @@
       <c r="D59" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E59" s="8"/>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="30"/>
+    <row r="60" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="42"/>
       <c r="B60" s="17" t="s">
         <v>98</v>
       </c>
@@ -3580,57 +3540,53 @@
       <c r="D60" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E60" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E60" s="8"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A61" s="30"/>
+    <row r="61" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="42"/>
       <c r="B61" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-    </row>
-    <row r="63" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A63" s="42" t="s">
+    <row r="62" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="45"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+    </row>
+    <row r="63" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A64" s="43"/>
+    <row r="64" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="53"/>
       <c r="B64" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="7"/>
-    </row>
-    <row r="65" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="43"/>
+      <c r="F64" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="53"/>
       <c r="B65" s="19" t="s">
         <v>102</v>
       </c>
@@ -3638,13 +3594,11 @@
       <c r="D65" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E65" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E65" s="8"/>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A66" s="43"/>
+    <row r="66" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="53"/>
       <c r="B66" s="19" t="s">
         <v>103</v>
       </c>
@@ -3652,13 +3606,11 @@
       <c r="D66" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E66" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E66" s="8"/>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A67" s="43"/>
+    <row r="67" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="53"/>
       <c r="B67" s="19" t="s">
         <v>104</v>
       </c>
@@ -3666,13 +3618,11 @@
       <c r="D67" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E67" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E67" s="8"/>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A68" s="43"/>
+    <row r="68" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="53"/>
       <c r="B68" s="19" t="s">
         <v>105</v>
       </c>
@@ -3680,97 +3630,89 @@
       <c r="D68" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E68" s="8"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A69" s="43"/>
+    <row r="69" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="53"/>
       <c r="B69" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="8"/>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A70" s="43"/>
+    <row r="70" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="53"/>
       <c r="B70" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="8"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A71" s="44"/>
-      <c r="B71" s="39" t="s">
+    <row r="71" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="54"/>
+      <c r="B71" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="8"/>
       <c r="F71" s="16"/>
     </row>
-    <row r="72" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1"/>
-    <row r="73" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1"/>
-    <row r="74" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1"/>
-    <row r="75" spans="1:6" ht="25.5">
-      <c r="A75" s="33" t="s">
+    <row r="72" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-    </row>
-    <row r="76" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B75" s="40"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="40"/>
+    </row>
+    <row r="76" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
+      <c r="B76" s="41"/>
+      <c r="C76" s="41"/>
       <c r="D76" s="4"/>
       <c r="E76" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F76" s="28"/>
     </row>
-    <row r="77" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
+    <row r="77" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="41"/>
+      <c r="B77" s="41"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="41"/>
       <c r="E77" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="78" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F78" s="7"/>
-    </row>
-    <row r="79" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="C78" s="44"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>53</v>
       </c>
@@ -3781,131 +3723,117 @@
       <c r="D79" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E79" s="8"/>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="80" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10"/>
       <c r="B80" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="8"/>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="81" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="10"/>
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C81" s="40"/>
-      <c r="D81" s="40"/>
-      <c r="E81" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="8"/>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="82" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="10"/>
-      <c r="B82" s="40" t="s">
+      <c r="B82" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C82" s="40"/>
-      <c r="D82" s="40"/>
-      <c r="E82" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="8"/>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="31"/>
-      <c r="C83" s="31"/>
-      <c r="D83" s="31"/>
-      <c r="E83" s="31"/>
-      <c r="F83" s="31"/>
-    </row>
-    <row r="84" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A84" s="30" t="s">
+    <row r="83" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="45"/>
+      <c r="B83" s="45"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+    </row>
+    <row r="84" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="8"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A85" s="30"/>
+    <row r="85" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="42"/>
       <c r="B85" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>149</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="E85" s="8"/>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A86" s="30"/>
-      <c r="B86" s="40" t="s">
+    <row r="86" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="42"/>
+      <c r="B86" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="8"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A87" s="30"/>
-      <c r="B87" s="40" t="s">
+    <row r="87" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="42"/>
+      <c r="B87" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="8"/>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A88" s="29"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
-    </row>
-    <row r="89" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A89" s="30" t="s">
+    <row r="88" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="37"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+    </row>
+    <row r="89" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="42" t="s">
         <v>26</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C89" s="45"/>
-      <c r="D89" s="45"/>
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
       <c r="E89" s="8"/>
-      <c r="F89" s="7"/>
-    </row>
-    <row r="90" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A90" s="30"/>
+      <c r="F89" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="42"/>
       <c r="B90" s="12" t="s">
         <v>62</v>
       </c>
@@ -3913,179 +3841,153 @@
       <c r="D90" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E90" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="E90" s="8"/>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A91" s="30"/>
+    <row r="91" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="42"/>
       <c r="B91" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C91" s="45"/>
-      <c r="D91" s="45"/>
-      <c r="E91" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C91" s="43"/>
+      <c r="D91" s="43"/>
+      <c r="E91" s="8"/>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A92" s="30"/>
+    <row r="92" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="42"/>
       <c r="B92" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C92" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="D92" s="47"/>
-      <c r="E92" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C92" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D92" s="50"/>
+      <c r="E92" s="8"/>
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A93" s="30"/>
+    <row r="93" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="42"/>
       <c r="B93" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C93" s="45"/>
-      <c r="D93" s="45"/>
-      <c r="E93" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="8"/>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A94" s="30"/>
+    <row r="94" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="42"/>
       <c r="B94" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C94" s="45"/>
-      <c r="D94" s="45"/>
-      <c r="E94" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C94" s="43"/>
+      <c r="D94" s="43"/>
+      <c r="E94" s="8"/>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A95" s="30"/>
-      <c r="B95" s="41" t="s">
+    <row r="95" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="42"/>
+      <c r="B95" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C95" s="41"/>
-      <c r="D95" s="41"/>
-      <c r="E95" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C95" s="46"/>
+      <c r="D95" s="46"/>
+      <c r="E95" s="8"/>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A96" s="30"/>
-      <c r="B96" s="41" t="s">
+    <row r="96" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="42"/>
+      <c r="B96" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C96" s="41"/>
-      <c r="D96" s="41"/>
-      <c r="E96" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C96" s="46"/>
+      <c r="D96" s="46"/>
+      <c r="E96" s="8"/>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A97" s="30"/>
+    <row r="97" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="42"/>
       <c r="B97" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C97" s="40"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="8"/>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A98" s="30"/>
+    <row r="98" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="42"/>
       <c r="B98" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C98" s="40"/>
-      <c r="D98" s="40"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
       <c r="E98" s="8"/>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A99" s="30"/>
-      <c r="B99" s="41" t="s">
+    <row r="99" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="42"/>
+      <c r="B99" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C99" s="41"/>
-      <c r="D99" s="41"/>
-      <c r="E99" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C99" s="46"/>
+      <c r="D99" s="46"/>
+      <c r="E99" s="8"/>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A100" s="30"/>
+    <row r="100" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="42"/>
       <c r="B100" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C100" s="40"/>
-      <c r="D100" s="40"/>
-      <c r="E100" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="8"/>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A101" s="30"/>
-      <c r="B101" s="41" t="s">
+    <row r="101" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="42"/>
+      <c r="B101" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C101" s="41"/>
-      <c r="D101" s="41"/>
-      <c r="E101" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C101" s="46"/>
+      <c r="D101" s="46"/>
+      <c r="E101" s="8"/>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A102" s="30"/>
+    <row r="102" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="42"/>
       <c r="B102" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C102" s="40"/>
-      <c r="D102" s="40"/>
-      <c r="E102" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C102" s="44"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="8"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A103" s="30"/>
-      <c r="B103" s="41" t="s">
+    <row r="103" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="42"/>
+      <c r="B103" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C103" s="41"/>
-      <c r="D103" s="41"/>
-      <c r="E103" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C103" s="46"/>
+      <c r="D103" s="46"/>
+      <c r="E103" s="8"/>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A104" s="30"/>
+    <row r="104" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="42"/>
       <c r="B104" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C104" s="45"/>
-      <c r="D104" s="45"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
       <c r="E104" s="8"/>
-      <c r="F104" s="7"/>
-    </row>
-    <row r="105" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A105" s="30"/>
+      <c r="F104" s="29"/>
+    </row>
+    <row r="105" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="42"/>
       <c r="B105" s="12" t="s">
         <v>77</v>
       </c>
@@ -4093,345 +3995,311 @@
       <c r="D105" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E105" s="8" t="s">
+      <c r="E105" s="8"/>
+      <c r="F105" s="7"/>
+    </row>
+    <row r="106" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="42"/>
+      <c r="B106" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C106" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="F105" s="7"/>
-    </row>
-    <row r="106" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A106" s="30"/>
-      <c r="B106" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C106" s="12" t="s">
-        <v>150</v>
-      </c>
       <c r="D106" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>149</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E106" s="8"/>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A107" s="30"/>
-      <c r="B107" s="41" t="s">
+    <row r="107" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="42"/>
+      <c r="B107" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C107" s="41"/>
-      <c r="D107" s="41"/>
-      <c r="E107" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C107" s="46"/>
+      <c r="D107" s="46"/>
+      <c r="E107" s="8"/>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A108" s="30"/>
-      <c r="B108" s="41" t="s">
+    <row r="108" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="42"/>
+      <c r="B108" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="C108" s="41"/>
-      <c r="D108" s="41"/>
-      <c r="E108" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C108" s="46"/>
+      <c r="D108" s="46"/>
+      <c r="E108" s="8"/>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A109" s="30"/>
-      <c r="B109" s="41" t="s">
+    <row r="109" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="42"/>
+      <c r="B109" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C109" s="41"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C109" s="46"/>
+      <c r="D109" s="46"/>
+      <c r="E109" s="8"/>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1"/>
-    <row r="111" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1"/>
-    <row r="112" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1"/>
-    <row r="113" spans="1:6" ht="26.1" customHeight="1">
-      <c r="A113" s="33" t="s">
+    <row r="110" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="1:6" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B113" s="33"/>
-      <c r="C113" s="33"/>
-      <c r="D113" s="33"/>
-      <c r="E113" s="33"/>
-      <c r="F113" s="33"/>
-    </row>
-    <row r="114" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
+      <c r="B113" s="40"/>
+      <c r="C113" s="40"/>
+      <c r="D113" s="40"/>
+      <c r="E113" s="40"/>
+      <c r="F113" s="40"/>
+    </row>
+    <row r="114" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B114" s="34"/>
-      <c r="C114" s="34"/>
+      <c r="B114" s="41"/>
+      <c r="C114" s="41"/>
       <c r="D114" s="4"/>
       <c r="E114" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F114" s="28"/>
     </row>
-    <row r="115" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A115" s="34"/>
-      <c r="B115" s="34"/>
-      <c r="C115" s="34"/>
-      <c r="D115" s="34"/>
+    <row r="115" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="41"/>
+      <c r="B115" s="41"/>
+      <c r="C115" s="41"/>
+      <c r="D115" s="41"/>
       <c r="E115" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A116" s="30" t="s">
+    <row r="116" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B116" s="48" t="s">
+      <c r="B116" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C116" s="49"/>
-      <c r="D116" s="50"/>
+      <c r="C116" s="31"/>
+      <c r="D116" s="32"/>
       <c r="E116" s="6"/>
       <c r="F116" s="7"/>
     </row>
-    <row r="117" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A117" s="30"/>
-      <c r="B117" s="36" t="s">
+    <row r="117" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="42"/>
+      <c r="B117" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C117" s="37"/>
-      <c r="D117" s="38"/>
-      <c r="E117" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C117" s="35"/>
+      <c r="D117" s="36"/>
+      <c r="E117" s="8"/>
       <c r="F117" s="7"/>
     </row>
-    <row r="118" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A118" s="30"/>
-      <c r="B118" s="45" t="s">
+    <row r="118" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="42"/>
+      <c r="B118" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="45"/>
-      <c r="D118" s="45"/>
-      <c r="E118" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C118" s="43"/>
+      <c r="D118" s="43"/>
+      <c r="E118" s="8"/>
       <c r="F118" s="7"/>
     </row>
-    <row r="119" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A119" s="30"/>
-      <c r="B119" s="36" t="s">
+    <row r="119" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="42"/>
+      <c r="B119" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C119" s="37"/>
-      <c r="D119" s="38"/>
-      <c r="E119" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C119" s="35"/>
+      <c r="D119" s="36"/>
+      <c r="E119" s="8"/>
       <c r="F119" s="7"/>
     </row>
-    <row r="120" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A120" s="30"/>
-      <c r="B120" s="36" t="s">
+    <row r="120" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="42"/>
+      <c r="B120" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C120" s="37"/>
-      <c r="D120" s="38"/>
-      <c r="E120" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C120" s="35"/>
+      <c r="D120" s="36"/>
+      <c r="E120" s="8"/>
       <c r="F120" s="7"/>
     </row>
-    <row r="121" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A121" s="30"/>
-      <c r="B121" s="48" t="s">
+    <row r="121" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="42"/>
+      <c r="B121" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C121" s="49"/>
-      <c r="D121" s="50"/>
+      <c r="C121" s="31"/>
+      <c r="D121" s="32"/>
       <c r="E121" s="8"/>
       <c r="F121" s="7"/>
     </row>
-    <row r="122" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A122" s="30"/>
-      <c r="B122" s="36" t="s">
+    <row r="122" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="42"/>
+      <c r="B122" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C122" s="37"/>
-      <c r="D122" s="38"/>
-      <c r="E122" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C122" s="35"/>
+      <c r="D122" s="36"/>
+      <c r="E122" s="8"/>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A123" s="30"/>
-      <c r="B123" s="36" t="s">
+    <row r="123" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="42"/>
+      <c r="B123" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C123" s="37"/>
-      <c r="D123" s="38"/>
-      <c r="E123" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C123" s="35"/>
+      <c r="D123" s="36"/>
+      <c r="E123" s="8"/>
       <c r="F123" s="7"/>
     </row>
-    <row r="124" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A124" s="30"/>
-      <c r="B124" s="36" t="s">
+    <row r="124" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="42"/>
+      <c r="B124" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C124" s="37"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C124" s="35"/>
+      <c r="D124" s="36"/>
+      <c r="E124" s="8"/>
       <c r="F124" s="7"/>
     </row>
-    <row r="125" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A125" s="30"/>
-      <c r="B125" s="36" t="s">
+    <row r="125" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="42"/>
+      <c r="B125" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C125" s="37"/>
-      <c r="D125" s="38"/>
-      <c r="E125" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C125" s="35"/>
+      <c r="D125" s="36"/>
+      <c r="E125" s="8"/>
       <c r="F125" s="7"/>
     </row>
-    <row r="126" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A126" s="30"/>
-      <c r="B126" s="36" t="s">
+    <row r="126" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="42"/>
+      <c r="B126" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C126" s="37"/>
-      <c r="D126" s="38"/>
-      <c r="E126" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C126" s="35"/>
+      <c r="D126" s="36"/>
+      <c r="E126" s="8"/>
       <c r="F126" s="7"/>
     </row>
-    <row r="127" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A127" s="30"/>
-      <c r="B127" s="36" t="s">
+    <row r="127" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="42"/>
+      <c r="B127" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C127" s="37"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C127" s="35"/>
+      <c r="D127" s="36"/>
+      <c r="E127" s="8"/>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A128" s="30"/>
-      <c r="B128" s="48" t="s">
+    <row r="128" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="42"/>
+      <c r="B128" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C128" s="49"/>
-      <c r="D128" s="50"/>
+      <c r="C128" s="31"/>
+      <c r="D128" s="32"/>
       <c r="E128" s="8"/>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A129" s="30"/>
-      <c r="B129" s="36" t="s">
+    <row r="129" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="42"/>
+      <c r="B129" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C129" s="37"/>
-      <c r="D129" s="38"/>
-      <c r="E129" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C129" s="35"/>
+      <c r="D129" s="36"/>
+      <c r="E129" s="8"/>
       <c r="F129" s="7"/>
     </row>
-    <row r="130" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A130" s="30"/>
-      <c r="B130" s="36" t="s">
+    <row r="130" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="42"/>
+      <c r="B130" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C130" s="37"/>
-      <c r="D130" s="38"/>
-      <c r="E130" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="C130" s="35"/>
+      <c r="D130" s="36"/>
+      <c r="E130" s="8"/>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A131" s="29"/>
-      <c r="B131" s="29"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="29"/>
-      <c r="E131" s="29"/>
-      <c r="F131" s="29"/>
-    </row>
-    <row r="132" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A132" s="52" t="s">
+    <row r="131" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="37"/>
+      <c r="B131" s="37"/>
+      <c r="C131" s="37"/>
+      <c r="D131" s="37"/>
+      <c r="E131" s="37"/>
+      <c r="F131" s="37"/>
+    </row>
+    <row r="132" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B132" s="53"/>
-      <c r="C132" s="53"/>
-      <c r="D132" s="53"/>
-      <c r="E132" s="53"/>
-      <c r="F132" s="53"/>
-    </row>
-    <row r="133" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A133" s="52"/>
-      <c r="B133" s="53"/>
-      <c r="C133" s="53"/>
-      <c r="D133" s="53"/>
-      <c r="E133" s="53"/>
-      <c r="F133" s="53"/>
-    </row>
-    <row r="134" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A134" s="52"/>
-      <c r="B134" s="53"/>
-      <c r="C134" s="53"/>
-      <c r="D134" s="53"/>
-      <c r="E134" s="53"/>
-      <c r="F134" s="53"/>
-    </row>
-    <row r="135" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A135" s="52"/>
-      <c r="B135" s="53"/>
-      <c r="C135" s="53"/>
-      <c r="D135" s="53"/>
-      <c r="E135" s="53"/>
-      <c r="F135" s="53"/>
-    </row>
-    <row r="136" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A136" s="52"/>
-      <c r="B136" s="53"/>
-      <c r="C136" s="53"/>
-      <c r="D136" s="53"/>
-      <c r="E136" s="53"/>
-      <c r="F136" s="53"/>
-    </row>
-    <row r="137" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A137" s="52"/>
-      <c r="B137" s="53"/>
-      <c r="C137" s="53"/>
-      <c r="D137" s="53"/>
-      <c r="E137" s="53"/>
-      <c r="F137" s="53"/>
-    </row>
-    <row r="138" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1"/>
-    <row r="139" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1"/>
-    <row r="140" spans="1:6" ht="21.95" customHeight="1">
+      <c r="B132" s="39"/>
+      <c r="C132" s="39"/>
+      <c r="D132" s="39"/>
+      <c r="E132" s="39"/>
+      <c r="F132" s="39"/>
+    </row>
+    <row r="133" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="38"/>
+      <c r="B133" s="39"/>
+      <c r="C133" s="39"/>
+      <c r="D133" s="39"/>
+      <c r="E133" s="39"/>
+      <c r="F133" s="39"/>
+    </row>
+    <row r="134" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="38"/>
+      <c r="B134" s="39"/>
+      <c r="C134" s="39"/>
+      <c r="D134" s="39"/>
+      <c r="E134" s="39"/>
+      <c r="F134" s="39"/>
+    </row>
+    <row r="135" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="38"/>
+      <c r="B135" s="39"/>
+      <c r="C135" s="39"/>
+      <c r="D135" s="39"/>
+      <c r="E135" s="39"/>
+      <c r="F135" s="39"/>
+    </row>
+    <row r="136" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="38"/>
+      <c r="B136" s="39"/>
+      <c r="C136" s="39"/>
+      <c r="D136" s="39"/>
+      <c r="E136" s="39"/>
+      <c r="F136" s="39"/>
+    </row>
+    <row r="137" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="38"/>
+      <c r="B137" s="39"/>
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="39"/>
+      <c r="F137" s="39"/>
+    </row>
+    <row r="138" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E140" s="51"/>
-      <c r="F140" s="51"/>
-    </row>
-    <row r="141" spans="1:6" ht="21.95" customHeight="1">
+      <c r="E140" s="33"/>
+      <c r="F140" s="33"/>
+    </row>
+    <row r="141" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>147</v>
       </c>
@@ -4442,92 +4310,13 @@
       <c r="D141" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E141" s="51" t="s">
+      <c r="E141" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="F141" s="51"/>
+      <c r="F141" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="95">
-    <mergeCell ref="B121:D121"/>
-    <mergeCell ref="E141:F141"/>
-    <mergeCell ref="E140:F140"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A132:A137"/>
-    <mergeCell ref="B132:F137"/>
-    <mergeCell ref="A115:D115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B124:D124"/>
-    <mergeCell ref="B126:D126"/>
-    <mergeCell ref="A116:A130"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="B123:D123"/>
-    <mergeCell ref="A89:A109"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="B129:D129"/>
-    <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B127:D127"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A63:A71"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B120:D120"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="A45:A53"/>
+  <mergeCells count="94">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A26:A38"/>
@@ -4544,6 +4333,84 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="A10:F10"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="A45:A53"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A63:A71"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A89:A109"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="A116:A130"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="B123:D123"/>
+    <mergeCell ref="B120:D120"/>
+    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="E141:F141"/>
+    <mergeCell ref="E140:F140"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A132:A137"/>
+    <mergeCell ref="B132:F137"/>
+    <mergeCell ref="B129:D129"/>
+    <mergeCell ref="B125:D125"/>
+    <mergeCell ref="B127:D127"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="B126:D126"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.51181102362204722" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -4553,12 +4420,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>